<commit_message>
Added more files from Albany Evening News
</commit_message>
<xml_diff>
--- a/public/filedata.xlsx
+++ b/public/filedata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xfore.000\Documents\Source\files.bsatroop53.com\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B37F09D-A9C1-4D02-BB76-DF004A2149C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6C28C2-C8B4-48F1-BA0B-EE8697B4CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="3780" windowWidth="15720" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Url</t>
   </si>
@@ -102,6 +102,42 @@
   </si>
   <si>
     <t>whispering wires</t>
+  </si>
+  <si>
+    <t>albany_evening_news_1936_jun_25_big_moose.pdf</t>
+  </si>
+  <si>
+    <t>Bake Appointed to Big Moose Staff</t>
+  </si>
+  <si>
+    <t>albany_evening_news_1936_sep_25_promotions.pdf</t>
+  </si>
+  <si>
+    <t>Boy Scouts Win New Promotions</t>
+  </si>
+  <si>
+    <t>fort orange council,court of honor,albert bleadow,peter andrew,thomas latham,christian gersch</t>
+  </si>
+  <si>
+    <t>big moose,thomas latham,donald paul</t>
+  </si>
+  <si>
+    <t>albany_evening_news_1937_jun_11_camp_sign_up.pdf</t>
+  </si>
+  <si>
+    <t>Boy Scout Camp Enrollment Gains</t>
+  </si>
+  <si>
+    <t>big moose,fort orange council,william grooten,thomas latham</t>
+  </si>
+  <si>
+    <t>albany_evening_news_1937_jun_29_camp_sign_up.pdf</t>
+  </si>
+  <si>
+    <t>Assistant Director Appointed For Camp</t>
+  </si>
+  <si>
+    <t>fort orange council,camp hawley,george corson,robert lawrence</t>
   </si>
 </sst>
 </file>
@@ -430,23 +466,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157CC0BA-17F6-488C-A444-7C6F2D391173}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="88" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -487,10 +523,10 @@
         <v>17</v>
       </c>
       <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
         <v>23</v>
-      </c>
-      <c r="N1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -521,10 +557,126 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
-        <v>21</v>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1936</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>1936</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>1937</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>1937</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>